<commit_message>
changes for multithreading and Evergreen captcha
</commit_message>
<xml_diff>
--- a/MultiProcess/Config.xlsx
+++ b/MultiProcess/Config.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_1316C0497132EE8518E2EE9163A1CD370770DBE3" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{35D8A120-EEE1-471A-A525-67CEF896D453}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,22 +40,22 @@
     <t>Write_OOCL</t>
   </si>
   <si>
-    <t>D:\blume-proj\OceanCarrierRPA\APL\ContainerInformation</t>
-  </si>
-  <si>
-    <t>D:\blume-proj\OceanCarrierRPA\CMACGM\ContainerInformation</t>
-  </si>
-  <si>
-    <t>D:\blume-proj\OceanCarrierRPA\Evergreen\ContainerInformation</t>
-  </si>
-  <si>
-    <t>D:\blume-proj\OceanCarrierRPA\OOCL\ContainerInformation</t>
+    <t>C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\OceanCarrierRPA\APL\ContainerInformation</t>
+  </si>
+  <si>
+    <t>C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\OceanCarrierRPA\CMACGM\ContainerInformation</t>
+  </si>
+  <si>
+    <t>C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\OceanCarrierRPA\Evergreen\ContainerInformation</t>
+  </si>
+  <si>
+    <t>C:\Users\pvanausdeln\OneDrive - Blume Global\UiPath\OceanCarrierRPA\OceanCarrierRPA\OOCL\ContainerInformation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -365,7 +366,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -373,6 +374,10 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>